<commit_message>
First pass through to gym 1 wokring
</commit_message>
<xml_diff>
--- a/data/PokemonBlackRun.xlsx
+++ b/data/PokemonBlackRun.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\VolundrAI\pokemon-nuzlocke-ai\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBE2F84C-D4AC-469E-8E22-6E7FA7FA9E98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9BD3104-E9DB-4D82-AE43-683E852AA14C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3090" yWindow="2415" windowWidth="28800" windowHeight="15435" activeTab="1" xr2:uid="{CB951569-D3D8-40FA-9299-7A41F1F0BE7C}"/>
+    <workbookView xWindow="4140" yWindow="3105" windowWidth="28800" windowHeight="15435" activeTab="2" xr2:uid="{CB951569-D3D8-40FA-9299-7A41F1F0BE7C}"/>
   </bookViews>
   <sheets>
     <sheet name="Run" sheetId="4" r:id="rId1"/>
@@ -522,13 +522,13 @@
     <t>001a</t>
   </si>
   <si>
-    <t>002b</t>
-  </si>
-  <si>
-    <t>003c</t>
-  </si>
-  <si>
     <t>LevelCap</t>
+  </si>
+  <si>
+    <t>001b</t>
+  </si>
+  <si>
+    <t>001c</t>
   </si>
 </sst>
 </file>
@@ -908,7 +908,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -928,7 +928,7 @@
         <v>156</v>
       </c>
       <c r="D1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1053,7 +1053,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C438ECFF-3815-4BD0-B5ED-596B2401FBF4}">
   <dimension ref="A1:BD24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="202" zoomScaleNormal="202" workbookViewId="0"/>
+    <sheetView zoomScale="202" zoomScaleNormal="202" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2214,8 +2216,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA276F34-80F0-448A-93AA-1E9DFD1276DC}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="256" zoomScaleNormal="256" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" zoomScale="256" zoomScaleNormal="256" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2277,7 +2279,7 @@
         <v>135</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D3" t="s">
         <v>67</v>
@@ -2298,7 +2300,7 @@
         <v>135</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D4" t="s">
         <v>5</v>

</xml_diff>